<commit_message>
Adding error messages and updating Initial migration
</commit_message>
<xml_diff>
--- a/Common/DataSchema/Schema.xlsx
+++ b/Common/DataSchema/Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMaestroRamirez\source\repos\TheMine\Common\DataSchema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMaestroRamirez\source\repos\DanielMaestro\Alessa\Common\DataSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEFBA4F-D55D-421E-B527-1A4B33B7F45E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C2E7A-E930-4E0A-B7FB-1FDF7839F75E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Alessa.TableConfiguration" sheetId="18" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alessa.FieldDefinition!$A$1:$I$85</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Alessa.FieldDefinitionUi!$A$1:$AB$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Alessa.FieldDefinitionUi!$A$1:$AF$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Alessa.FieldKeysRelationship!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Alessa.TableDefinition!$A$1:$E$1</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="324">
   <si>
     <t>ItemName</t>
   </si>
@@ -1086,6 +1086,18 @@
   </si>
   <si>
     <t>AfterCreate</t>
+  </si>
+  <si>
+    <t>RequiredErrorMsg</t>
+  </si>
+  <si>
+    <t>RegexErrorMsg</t>
+  </si>
+  <si>
+    <t>MinLengthErrorMsg</t>
+  </si>
+  <si>
+    <t>MaxLengthErrorMsg</t>
   </si>
 </sst>
 </file>
@@ -4689,7 +4701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB104D6-C294-4D4F-9258-F7A2971580B6}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -7367,12 +7379,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BCF39D-315F-4810-8B54-5D5D18B35E09}">
-  <dimension ref="A1:AB85"/>
+  <dimension ref="A1:AF85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="R35" sqref="R35"/>
+      <selection pane="bottomLeft" activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7392,10 +7404,10 @@
     <col min="20" max="21" width="7.28515625" style="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.42578125" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" customWidth="1"/>
+    <col min="24" max="28" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
@@ -7469,19 +7481,31 @@
         <v>160</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7545,16 +7569,28 @@
         <v>18</v>
       </c>
       <c r="Z2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>VLOOKUP($G3,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7572,11 +7608,11 @@
         <v>Integer</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB3,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF3,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB3,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF3,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G3" s="1">
@@ -7645,8 +7681,20 @@
       <c r="AB3" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>VLOOKUP($G4,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7664,11 +7712,11 @@
         <v>Text</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB4,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF4,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB4,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF4,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G4" s="1">
@@ -7737,8 +7785,20 @@
       <c r="AB4" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>VLOOKUP($G5,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7756,11 +7816,11 @@
         <v>Text</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB5,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF5,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB5,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF5,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G5" s="1">
@@ -7829,8 +7889,20 @@
       <c r="AB5" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>VLOOKUP($G6,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7848,11 +7920,11 @@
         <v>Bit</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB6,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF6,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB6,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF6,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G6" s="1">
@@ -7921,8 +7993,20 @@
       <c r="AB6" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>VLOOKUP($G7,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -7940,11 +8024,11 @@
         <v>Integer</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB7,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF7,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB7,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF7,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G7" s="1">
@@ -8013,8 +8097,20 @@
       <c r="AB7" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>VLOOKUP($G8,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8032,11 +8128,11 @@
         <v>Bit</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB8,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF8,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB8,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF8,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G8" s="1">
@@ -8105,8 +8201,20 @@
       <c r="AB8" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>VLOOKUP($G9,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8124,11 +8232,11 @@
         <v>Integer</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB9,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF9,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB9,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF9,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G9" s="1">
@@ -8197,8 +8305,20 @@
       <c r="AB9" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>VLOOKUP($G10,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8216,11 +8336,11 @@
         <v>Text</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB10,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF10,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB10,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF10,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G10" s="1">
@@ -8289,8 +8409,20 @@
       <c r="AB10" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>VLOOKUP($G11,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8308,11 +8440,11 @@
         <v>Text</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB11,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF11,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB11,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF11,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G11" s="1">
@@ -8381,8 +8513,20 @@
       <c r="AB11" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>VLOOKUP($G12,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8400,11 +8544,11 @@
         <v>Bit</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB12,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF12,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB12,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF12,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G12" s="1">
@@ -8473,8 +8617,20 @@
       <c r="AB12" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>VLOOKUP($G13,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8492,11 +8648,11 @@
         <v>Text</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB13,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF13,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB13,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF13,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G13" s="1">
@@ -8556,17 +8712,29 @@
       <c r="Y13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="1">
+      <c r="Z13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="1">
         <v>12</v>
       </c>
-      <c r="AB13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>VLOOKUP($G14,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8584,11 +8752,11 @@
         <v>Bit</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB14,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF14,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB14,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF14,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G14" s="1">
@@ -8648,17 +8816,29 @@
       <c r="Y14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="1">
+      <c r="Z14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="1">
         <v>12</v>
       </c>
-      <c r="AB14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>VLOOKUP($G15,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8676,11 +8856,11 @@
         <v>Date</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB15,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF15,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB15,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF15,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G15" s="1">
@@ -8740,17 +8920,29 @@
       <c r="Y15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z15" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="1">
+      <c r="Z15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="1">
         <v>12</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AF15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>VLOOKUP($G16,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8768,11 +8960,11 @@
         <v>DateTime</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB16,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF16,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB16,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF16,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G16" s="1">
@@ -8832,17 +9024,29 @@
       <c r="Y16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="1">
+      <c r="Z16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="1">
         <v>12</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AF16" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>VLOOKUP($G17,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8860,11 +9064,11 @@
         <v>Decimal</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB17,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF17,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB17,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF17,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G17" s="1">
@@ -8924,17 +9128,29 @@
       <c r="Y17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="1">
+      <c r="Z17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="1">
         <v>12</v>
       </c>
-      <c r="AB17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>VLOOKUP($G18,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8952,11 +9168,11 @@
         <v>Integer</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB18,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF18,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB18,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF18,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G18" s="1">
@@ -9016,17 +9232,29 @@
       <c r="Y18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="1">
+      <c r="Z18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="1">
         <v>12</v>
       </c>
-      <c r="AB18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>VLOOKUP($G19,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9044,11 +9272,11 @@
         <v>Decimal</v>
       </c>
       <c r="E19" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB19,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF19,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB19,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF19,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G19" s="1">
@@ -9108,17 +9336,29 @@
       <c r="Y19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z19" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="1">
+      <c r="Z19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="1">
         <v>12</v>
       </c>
-      <c r="AB19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AF19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f>VLOOKUP($G20,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9136,11 +9376,11 @@
         <v>RichText</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB20,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF20,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB20,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF20,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G20" s="1">
@@ -9200,17 +9440,29 @@
       <c r="Y20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="1">
+      <c r="Z20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="1">
         <v>12</v>
       </c>
-      <c r="AB20" s="1">
+      <c r="AF20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>VLOOKUP($G21,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9228,11 +9480,11 @@
         <v>Text</v>
       </c>
       <c r="E21" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB21,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF21,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB21,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF21,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G21" s="1">
@@ -9292,17 +9544,29 @@
       <c r="Y21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="1">
+      <c r="Z21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE21" s="1">
         <v>12</v>
       </c>
-      <c r="AB21" s="1">
+      <c r="AF21" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f>VLOOKUP($G22,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9320,11 +9584,11 @@
         <v>TextArea</v>
       </c>
       <c r="E22" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB22,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF22,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB22,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF22,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G22" s="1">
@@ -9384,17 +9648,29 @@
       <c r="Y22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z22" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="1">
+      <c r="Z22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE22" s="1">
         <v>12</v>
       </c>
-      <c r="AB22" s="1">
+      <c r="AF22" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f>VLOOKUP($G23,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9412,11 +9688,11 @@
         <v>Time</v>
       </c>
       <c r="E23" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB23,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF23,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB23,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF23,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G23" s="1">
@@ -9476,17 +9752,29 @@
       <c r="Y23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="1">
+      <c r="Z23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="1">
         <v>12</v>
       </c>
-      <c r="AB23" s="1">
+      <c r="AF23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f>VLOOKUP($G24,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9504,11 +9792,11 @@
         <v>Integer</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB24,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF24,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB24,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF24,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G24" s="1">
@@ -9577,8 +9865,20 @@
       <c r="AB24" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f>VLOOKUP($G25,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9596,11 +9896,11 @@
         <v>Text</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB25,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF25,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB25,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF25,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G25" s="1">
@@ -9669,8 +9969,20 @@
       <c r="AB25" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>VLOOKUP($G26,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9688,11 +10000,11 @@
         <v>DateTime</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB26,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF26,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB26,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF26,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G26" s="1">
@@ -9761,8 +10073,20 @@
       <c r="AB26" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>VLOOKUP($G27,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9780,11 +10104,11 @@
         <v>Integer</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB27,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF27,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB27,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF27,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G27" s="1">
@@ -9853,8 +10177,20 @@
       <c r="AB27" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f>VLOOKUP($G28,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9872,11 +10208,11 @@
         <v>Integer</v>
       </c>
       <c r="E28" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB28,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF28,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB28,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF28,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G28" s="1">
@@ -9945,8 +10281,20 @@
       <c r="AB28" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f>VLOOKUP($G29,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9964,11 +10312,11 @@
         <v>Bit</v>
       </c>
       <c r="E29" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB29,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF29,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB29,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF29,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G29" s="1">
@@ -10037,8 +10385,20 @@
       <c r="AB29" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>VLOOKUP($G30,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10056,11 +10416,11 @@
         <v>Bit</v>
       </c>
       <c r="E30" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB30,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF30,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB30,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF30,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G30" s="1">
@@ -10129,8 +10489,20 @@
       <c r="AB30" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>VLOOKUP($G31,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10148,11 +10520,11 @@
         <v>SingleSelect</v>
       </c>
       <c r="E31" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB31,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF31,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB31,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF31,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>List</v>
       </c>
       <c r="G31" s="1">
@@ -10212,17 +10584,29 @@
       <c r="Y31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA31" s="1">
+      <c r="Z31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="1">
         <v>12</v>
       </c>
-      <c r="AB31" s="1">
+      <c r="AF31" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>VLOOKUP($G32,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10240,11 +10624,11 @@
         <v>Text</v>
       </c>
       <c r="E32" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB32,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF32,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB32,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF32,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G32" s="1">
@@ -10304,17 +10688,29 @@
       <c r="Y32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z32" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="1">
+      <c r="Z32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE32" s="1">
         <v>12</v>
       </c>
-      <c r="AB32" s="1">
+      <c r="AF32" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>VLOOKUP($G33,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10332,11 +10728,11 @@
         <v>DateTime</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB33,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF33,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB33,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF33,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G33" s="1">
@@ -10396,17 +10792,29 @@
       <c r="Y33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="1">
+      <c r="Z33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="1">
         <v>12</v>
       </c>
-      <c r="AB33" s="1">
+      <c r="AF33" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>VLOOKUP($G34,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10424,11 +10832,11 @@
         <v>Integer</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB34,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF34,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB34,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF34,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G34" s="1">
@@ -10488,17 +10896,29 @@
       <c r="Y34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="1">
+      <c r="Z34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="1">
         <v>12</v>
       </c>
-      <c r="AB34" s="1">
+      <c r="AF34" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>VLOOKUP($G35,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10516,11 +10936,11 @@
         <v>Radio</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB35,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF35,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB35,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF35,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Radio</v>
       </c>
       <c r="G35" s="1">
@@ -10580,17 +11000,29 @@
       <c r="Y35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA35" s="1">
+      <c r="Z35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="1">
         <v>12</v>
       </c>
-      <c r="AB35" s="1">
+      <c r="AF35" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f>VLOOKUP($G36,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -10608,11 +11040,11 @@
         <v>Integer</v>
       </c>
       <c r="E36" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB36,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF36,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB36,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF36,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G36" s="1">
@@ -10681,8 +11113,20 @@
       <c r="AB36" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>VLOOKUP($G37,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -10700,11 +11144,11 @@
         <v>Bit</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB37,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF37,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB37,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF37,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G37" s="1">
@@ -10773,8 +11217,20 @@
       <c r="AB37" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f>VLOOKUP($G38,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -10792,11 +11248,11 @@
         <v>Text</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB38,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF38,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB38,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF38,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G38" s="1">
@@ -10865,8 +11321,20 @@
       <c r="AB38" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF38" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f>VLOOKUP($G39,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -10884,11 +11352,11 @@
         <v>Bit</v>
       </c>
       <c r="E39" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB39,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF39,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB39,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF39,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G39" s="1">
@@ -10948,17 +11416,29 @@
       <c r="Y39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA39" s="1">
+      <c r="Z39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE39" s="1">
         <v>12</v>
       </c>
-      <c r="AB39" s="1">
+      <c r="AF39" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f>VLOOKUP($G40,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -10976,11 +11456,11 @@
         <v>Text</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB40,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF40,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB40,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF40,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G40" s="1">
@@ -11040,17 +11520,29 @@
       <c r="Y40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA40" s="1">
+      <c r="Z40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE40" s="1">
         <v>12</v>
       </c>
-      <c r="AB40" s="1">
+      <c r="AF40" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f>VLOOKUP($G41,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11068,11 +11560,11 @@
         <v>Decimal</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB41,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF41,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB41,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF41,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G41" s="1">
@@ -11132,17 +11624,29 @@
       <c r="Y41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA41" s="1">
+      <c r="Z41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE41" s="1">
         <v>12</v>
       </c>
-      <c r="AB41" s="1">
+      <c r="AF41" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f>VLOOKUP($G42,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11160,11 +11664,11 @@
         <v>Text</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB42,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF42,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB42,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF42,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Furthermore</v>
       </c>
       <c r="G42" s="1">
@@ -11224,17 +11728,29 @@
       <c r="Y42" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA42" s="1">
+      <c r="Z42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="1">
         <v>12</v>
       </c>
-      <c r="AB42" s="1">
+      <c r="AF42" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f>VLOOKUP($G43,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11252,11 +11768,11 @@
         <v>MultiselectList</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB43,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF43,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB43,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF43,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G43" s="1">
@@ -11316,17 +11832,29 @@
       <c r="Y43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA43" s="1">
+      <c r="Z43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE43" s="1">
         <v>12</v>
       </c>
-      <c r="AB43" s="1">
+      <c r="AF43" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f>VLOOKUP($G44,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11344,11 +11872,11 @@
         <v>Text</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB44,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF44,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB44,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF44,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G44" s="1">
@@ -11408,17 +11936,29 @@
       <c r="Y44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA44" s="1">
+      <c r="Z44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="1">
         <v>12</v>
       </c>
-      <c r="AB44" s="1">
+      <c r="AF44" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f>VLOOKUP($G45,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11436,11 +11976,11 @@
         <v>Text</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB45,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF45,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB45,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF45,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Furthermore</v>
       </c>
       <c r="G45" s="1">
@@ -11500,17 +12040,29 @@
       <c r="Y45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA45" s="1">
+      <c r="Z45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE45" s="1">
         <v>12</v>
       </c>
-      <c r="AB45" s="1">
+      <c r="AF45" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f>VLOOKUP($G46,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11528,11 +12080,11 @@
         <v>Text</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB46,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF46,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB46,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF46,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G46" s="1">
@@ -11592,17 +12144,29 @@
       <c r="Y46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z46" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA46" s="1">
+      <c r="Z46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="1">
         <v>12</v>
       </c>
-      <c r="AB46" s="1">
+      <c r="AF46" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f>VLOOKUP($G47,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -11620,11 +12184,11 @@
         <v>Bit</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB47,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF47,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB47,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF47,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G47" s="1">
@@ -11693,8 +12257,20 @@
       <c r="AB47" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF47" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>VLOOKUP($G48,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -11712,11 +12288,11 @@
         <v>Text</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB48,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF48,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB48,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF48,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G48" s="1">
@@ -11785,8 +12361,20 @@
       <c r="AB48" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF48" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f>VLOOKUP($G49,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -11804,11 +12392,11 @@
         <v>Integer</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB49,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF49,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB49,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF49,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G49" s="1">
@@ -11877,8 +12465,20 @@
       <c r="AB49" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF49" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f>VLOOKUP($G50,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -11896,11 +12496,11 @@
         <v>Decimal</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB50,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF50,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB50,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF50,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G50" s="1">
@@ -11969,8 +12569,20 @@
       <c r="AB50" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF50" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f>VLOOKUP($G51,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -11988,11 +12600,11 @@
         <v>Text</v>
       </c>
       <c r="E51" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB51,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF51,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB51,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF51,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G51" s="1">
@@ -12061,8 +12673,20 @@
       <c r="AB51" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF51" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f>VLOOKUP($G52,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12080,11 +12704,11 @@
         <v>Text</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB52,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF52,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB52,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF52,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G52" s="1">
@@ -12153,8 +12777,20 @@
       <c r="AB52" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF52" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f>VLOOKUP($G53,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12172,11 +12808,11 @@
         <v>Text</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB53,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF53,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB53,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF53,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G53" s="1">
@@ -12245,8 +12881,20 @@
       <c r="AB53" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF53" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f>VLOOKUP($G54,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12264,11 +12912,11 @@
         <v>Bit</v>
       </c>
       <c r="E54" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB54,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF54,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB54,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF54,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G54" s="1">
@@ -12337,8 +12985,20 @@
       <c r="AB54" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF54" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f>VLOOKUP($G55,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12356,11 +13016,11 @@
         <v>Bit</v>
       </c>
       <c r="E55" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB55,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF55,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB55,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF55,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G55" s="1">
@@ -12429,8 +13089,20 @@
       <c r="AB55" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF55" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f>VLOOKUP($G56,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -12448,11 +13120,11 @@
         <v>Integer</v>
       </c>
       <c r="E56" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB56,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF56,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB56,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF56,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G56" s="1">
@@ -12521,8 +13193,20 @@
       <c r="AB56" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF56" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f>VLOOKUP($G57,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -12540,11 +13224,11 @@
         <v>Bit</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB57,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF57,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB57,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF57,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G57" s="1">
@@ -12613,8 +13297,20 @@
       <c r="AB57" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF57" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f>VLOOKUP($G58,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -12632,11 +13328,11 @@
         <v>Integer</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB58,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF58,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB58,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF58,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G58" s="1">
@@ -12705,8 +13401,20 @@
       <c r="AB58" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF58" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f>VLOOKUP($G59,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -12724,11 +13432,11 @@
         <v>Integer</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB59,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF59,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB59,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF59,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G59" s="1">
@@ -12797,8 +13505,20 @@
       <c r="AB59" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF59" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f>VLOOKUP($G60,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -12816,11 +13536,11 @@
         <v>Bit</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB60,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF60,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB60,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF60,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G60" s="1">
@@ -12889,8 +13609,20 @@
       <c r="AB60" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF60" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f>VLOOKUP($G61,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -12908,11 +13640,11 @@
         <v>Integer</v>
       </c>
       <c r="E61" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB61,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF61,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB61,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF61,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G61" s="1">
@@ -12981,8 +13713,20 @@
       <c r="AB61" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF61" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f>VLOOKUP($G62,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>11</v>
@@ -13000,11 +13744,11 @@
         <v>DateTime</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB62,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF62,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB62,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF62,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G62" s="1">
@@ -13073,8 +13817,20 @@
       <c r="AB62" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF62" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>VLOOKUP($G63,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>11</v>
@@ -13092,11 +13848,11 @@
         <v>Integer</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB63,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF63,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB63,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF63,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G63" s="1">
@@ -13165,8 +13921,20 @@
       <c r="AB63" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f>VLOOKUP($G64,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13184,11 +13952,11 @@
         <v>MultiselectCheckbox</v>
       </c>
       <c r="E64" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB64,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF64,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB64,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF64,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>MultiCheckbox</v>
       </c>
       <c r="G64" s="1">
@@ -13248,17 +14016,29 @@
       <c r="Y64" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z64" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA64" s="1">
+      <c r="Z64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD64" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE64" s="1">
         <v>12</v>
       </c>
-      <c r="AB64" s="1">
+      <c r="AF64" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f>VLOOKUP($G65,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13276,11 +14056,11 @@
         <v>DateTime</v>
       </c>
       <c r="E65" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB65,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF65,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB65,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF65,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CommonData</v>
       </c>
       <c r="G65" s="1">
@@ -13340,17 +14120,29 @@
       <c r="Y65" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z65" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA65" s="1">
+      <c r="Z65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD65" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE65" s="1">
         <v>12</v>
       </c>
-      <c r="AB65" s="1">
+      <c r="AF65" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f>VLOOKUP($G66,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13368,11 +14160,11 @@
         <v>MultiselectList</v>
       </c>
       <c r="E66" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB66,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF66,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB66,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF66,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>MultiSelect</v>
       </c>
       <c r="G66" s="1">
@@ -13432,17 +14224,29 @@
       <c r="Y66" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z66" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA66" s="1">
+      <c r="Z66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD66" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE66" s="1">
         <v>12</v>
       </c>
-      <c r="AB66" s="1">
+      <c r="AF66" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f>VLOOKUP($G67,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13460,11 +14264,11 @@
         <v>Integer</v>
       </c>
       <c r="E67" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB67,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF67,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB67,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF67,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CommonData</v>
       </c>
       <c r="G67" s="1">
@@ -13524,17 +14328,29 @@
       <c r="Y67" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z67" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA67" s="1">
+      <c r="Z67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD67" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE67" s="1">
         <v>12</v>
       </c>
-      <c r="AB67" s="1">
+      <c r="AF67" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f>VLOOKUP($G68,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13552,11 +14368,11 @@
         <v>TableReference</v>
       </c>
       <c r="E68" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB68,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF68,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB68,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF68,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Grid</v>
       </c>
       <c r="G68" s="1">
@@ -13616,17 +14432,29 @@
       <c r="Y68" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z68" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA68" s="1">
+      <c r="Z68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD68" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE68" s="1">
         <v>12</v>
       </c>
-      <c r="AB68" s="1">
+      <c r="AF68" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f>VLOOKUP($G69,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -13644,11 +14472,11 @@
         <v>Text</v>
       </c>
       <c r="E69" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB69,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF69,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB69,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF69,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G69" s="1">
@@ -13717,8 +14545,20 @@
       <c r="AB69" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF69" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f>VLOOKUP($G70,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -13736,11 +14576,11 @@
         <v>Bit</v>
       </c>
       <c r="E70" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB70,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF70,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB70,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF70,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G70" s="1">
@@ -13809,8 +14649,20 @@
       <c r="AB70" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF70" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f>VLOOKUP($G71,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -13828,11 +14680,11 @@
         <v>Integer</v>
       </c>
       <c r="E71" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB71,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF71,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB71,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF71,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G71" s="1">
@@ -13901,8 +14753,20 @@
       <c r="AB71" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF71" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f>VLOOKUP($G72,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -13920,11 +14784,11 @@
         <v>Integer</v>
       </c>
       <c r="E72" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB72,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF72,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB72,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF72,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G72" s="1">
@@ -13984,17 +14848,29 @@
       <c r="Y72" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z72" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA72" s="1">
+      <c r="Z72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD72" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE72" s="1">
         <v>12</v>
       </c>
-      <c r="AB72" s="1">
+      <c r="AF72" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f>VLOOKUP($G73,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14012,11 +14888,11 @@
         <v>DateTime</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB73,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF73,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB73,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF73,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G73" s="1">
@@ -14076,17 +14952,29 @@
       <c r="Y73" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z73" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA73" s="1">
+      <c r="Z73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE73" s="1">
         <v>12</v>
       </c>
-      <c r="AB73" s="1">
+      <c r="AF73" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f>VLOOKUP($G74,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14104,11 +14992,11 @@
         <v>Integer</v>
       </c>
       <c r="E74" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB74,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF74,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB74,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF74,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G74" s="1">
@@ -14168,17 +15056,29 @@
       <c r="Y74" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z74" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA74" s="1">
+      <c r="Z74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD74" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE74" s="1">
         <v>12</v>
       </c>
-      <c r="AB74" s="1">
+      <c r="AF74" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f>VLOOKUP($G75,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14196,11 +15096,11 @@
         <v>Integer</v>
       </c>
       <c r="E75" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB75,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF75,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB75,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF75,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G75" s="1">
@@ -14260,17 +15160,29 @@
       <c r="Y75" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z75" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA75" s="1">
+      <c r="Z75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD75" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE75" s="1">
         <v>12</v>
       </c>
-      <c r="AB75" s="1">
+      <c r="AF75" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f>VLOOKUP($G76,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14288,11 +15200,11 @@
         <v>Text</v>
       </c>
       <c r="E76" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB76,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF76,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB76,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF76,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G76" s="1">
@@ -14352,17 +15264,29 @@
       <c r="Y76" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z76" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA76" s="1">
+      <c r="Z76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD76" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE76" s="1">
         <v>12</v>
       </c>
-      <c r="AB76" s="1">
+      <c r="AF76" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>VLOOKUP($G77,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14380,11 +15304,11 @@
         <v>Text</v>
       </c>
       <c r="E77" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB77,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF77,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB77,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF77,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G77" s="1">
@@ -14444,17 +15368,29 @@
       <c r="Y77" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z77" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA77" s="1">
+      <c r="Z77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD77" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE77" s="1">
         <v>12</v>
       </c>
-      <c r="AB77" s="1">
+      <c r="AF77" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f>VLOOKUP($G78,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14472,11 +15408,11 @@
         <v>DateTime</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB78,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF78,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB78,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF78,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G78" s="1">
@@ -14536,17 +15472,29 @@
       <c r="Y78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z78" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA78" s="1">
+      <c r="Z78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD78" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE78" s="1">
         <v>12</v>
       </c>
-      <c r="AB78" s="1">
+      <c r="AF78" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f>VLOOKUP($G79,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14564,11 +15512,11 @@
         <v>Text</v>
       </c>
       <c r="E79" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB79,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF79,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB79,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF79,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G79" s="1">
@@ -14628,17 +15576,29 @@
       <c r="Y79" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z79" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA79" s="1">
+      <c r="Z79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE79" s="1">
         <v>12</v>
       </c>
-      <c r="AB79" s="1">
+      <c r="AF79" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f>VLOOKUP($G80,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14656,11 +15616,11 @@
         <v>Text</v>
       </c>
       <c r="E80" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB80,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF80,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB80,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF80,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G80" s="1">
@@ -14720,17 +15680,29 @@
       <c r="Y80" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z80" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA80" s="1">
+      <c r="Z80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD80" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE80" s="1">
         <v>12</v>
       </c>
-      <c r="AB80" s="1">
+      <c r="AF80" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f>VLOOKUP($G81,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -14748,11 +15720,11 @@
         <v>Integer</v>
       </c>
       <c r="E81" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB81,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF81,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB81,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF81,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G81" s="1">
@@ -14812,17 +15784,29 @@
       <c r="Y81" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z81" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA81" s="1">
+      <c r="Z81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD81" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE81" s="1">
         <v>12</v>
       </c>
-      <c r="AB81" s="1">
+      <c r="AF81" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f>VLOOKUP($G82,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -14840,11 +15824,11 @@
         <v>Text</v>
       </c>
       <c r="E82" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB82,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF82,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB82,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF82,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G82" s="1">
@@ -14904,17 +15888,29 @@
       <c r="Y82" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z82" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA82" s="1">
+      <c r="Z82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD82" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE82" s="1">
         <v>12</v>
       </c>
-      <c r="AB82" s="1">
+      <c r="AF82" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f>VLOOKUP($G83,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -14932,11 +15928,11 @@
         <v>Text</v>
       </c>
       <c r="E83" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB83,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF83,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB83,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF83,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G83" s="1">
@@ -14996,17 +15992,29 @@
       <c r="Y83" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z83" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA83" s="1">
+      <c r="Z83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD83" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE83" s="1">
         <v>12</v>
       </c>
-      <c r="AB83" s="1">
+      <c r="AF83" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f>VLOOKUP($G84,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -15024,11 +16032,11 @@
         <v>Bit</v>
       </c>
       <c r="E84" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB84,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF84,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB84,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF84,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G84" s="1">
@@ -15088,17 +16096,29 @@
       <c r="Y84" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z84" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA84" s="1">
+      <c r="Z84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD84" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE84" s="1">
         <v>12</v>
       </c>
-      <c r="AB84" s="1">
+      <c r="AF84" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f>VLOOKUP($G85,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -15116,11 +16136,11 @@
         <v>TableReference</v>
       </c>
       <c r="E85" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AB85,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AF85,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AB85,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AF85,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CatalogTypes</v>
       </c>
       <c r="G85" s="1">
@@ -15180,18 +16200,30 @@
       <c r="Y85" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z85" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA85" s="1">
+      <c r="Z85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD85" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE85" s="1">
         <v>12</v>
       </c>
-      <c r="AB85" s="1">
+      <c r="AF85" s="1">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB85" xr:uid="{98088FFF-07F4-4BB5-BAC5-BF377CA38131}"/>
+  <autoFilter ref="A1:AF85" xr:uid="{98088FFF-07F4-4BB5-BAC5-BF377CA38131}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added On enter Create event method.
</commit_message>
<xml_diff>
--- a/Common/DataSchema/Schema.xlsx
+++ b/Common/DataSchema/Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMaestroRamirez\source\repos\DanielMaestro\Alessa\Common\DataSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C2E7A-E930-4E0A-B7FB-1FDF7839F75E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A8D2BC-7F8A-4515-81DA-8E1FE7C688C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Alessa.TableConfiguration" sheetId="18" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="326">
   <si>
     <t>ItemName</t>
   </si>
@@ -521,9 +521,6 @@
   </si>
   <si>
     <t>TextArea</t>
-  </si>
-  <si>
-    <t>BeforeCreate</t>
   </si>
   <si>
     <t>Is Commited</t>
@@ -1098,6 +1095,15 @@
   </si>
   <si>
     <t>MaxLengthErrorMsg</t>
+  </si>
+  <si>
+    <t>OnEnterCreate</t>
+  </si>
+  <si>
+    <t>Default values for HideEnableSample</t>
+  </si>
+  <si>
+    <t>From(Samples.HideEnableSample) Select(25 AS HideWhen2OrMore, 'Record {{HideEnableSampleId}}' AS EnableWhen5) Limit(1)</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1474,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1493,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1501,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1503,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1544,7 +1550,7 @@
         <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>119</v>
@@ -1594,7 +1600,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>59</v>
@@ -1624,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>62</v>
@@ -1840,7 +1846,7 @@
         <v>140</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2833,16 +2839,16 @@
         <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2885,7 +2891,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2911,7 +2917,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2937,7 +2943,7 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2963,7 +2969,7 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2989,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3015,7 +3021,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3025,10 +3031,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC13036-1340-4025-9566-920D3F8AF350}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3038,19 +3044,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3078,10 +3084,10 @@
         <v>105</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E3" s="1">
         <v>2</v>
@@ -3095,10 +3101,10 @@
         <v>105</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -3112,10 +3118,10 @@
         <v>105</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -3129,10 +3135,10 @@
         <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -3146,10 +3152,10 @@
         <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -3163,10 +3169,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -3180,10 +3186,10 @@
         <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -3197,10 +3203,10 @@
         <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -3214,10 +3220,10 @@
         <v>105</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -3231,10 +3237,10 @@
         <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -3248,10 +3254,10 @@
         <v>105</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -3265,10 +3271,10 @@
         <v>105</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -3282,10 +3288,10 @@
         <v>105</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -3296,13 +3302,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="2" t="s">
         <v>174</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -3313,13 +3319,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -3333,12 +3339,29 @@
         <v>105</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="E18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E19" s="1">
         <v>2</v>
       </c>
     </row>
@@ -3362,10 +3385,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -3387,7 +3410,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -3410,25 +3433,25 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>251</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -3465,22 +3488,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H3" s="1">
         <v>1</v>
@@ -3531,7 +3554,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -3559,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>128</v>
@@ -3579,7 +3602,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>129</v>
@@ -3599,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>130</v>
@@ -3619,10 +3642,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>286</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>107</v>
@@ -3639,10 +3662,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>287</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>108</v>
@@ -3659,7 +3682,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>131</v>
@@ -3679,10 +3702,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>290</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>291</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>108</v>
@@ -3699,10 +3722,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>107</v>
@@ -3719,7 +3742,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>132</v>
@@ -3739,7 +3762,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>133</v>
@@ -3759,10 +3782,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>296</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>107</v>
@@ -3779,10 +3802,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>108</v>
@@ -3799,7 +3822,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>134</v>
@@ -3819,10 +3842,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>107</v>
@@ -3903,28 +3926,28 @@
         <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>315</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>137</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -4113,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -4209,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -4305,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4545,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -4641,7 +4664,7 @@
         <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -4689,7 +4712,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
   </sheetData>
@@ -4699,10 +4722,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB104D6-C294-4D4F-9258-F7A2971580B6}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4720,13 +4743,13 @@
         <v>102</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -4756,7 +4779,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>154</v>
+        <v>323</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -4774,7 +4797,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>154</v>
+        <v>323</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
@@ -4789,12 +4812,30 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E5" s="1">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>VLOOKUP($B6,Alessa.TableDefinition!$A$3:$F$17,2)</f>
+        <v>Samples.HideEnableSamplesView</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4843,7 +4884,7 @@
         <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>99</v>
@@ -5703,7 +5744,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
@@ -6453,7 +6494,7 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E55" s="1">
         <v>0</v>
@@ -7381,10 +7422,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BCF39D-315F-4810-8B54-5D5D18B35E09}">
   <dimension ref="A1:AF85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="Z18" sqref="Z18"/>
+      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7421,10 +7462,10 @@
         <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>104</v>
@@ -7433,13 +7474,13 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>180</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -7454,10 +7495,10 @@
         <v>137</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>149</v>
@@ -7466,43 +7507,43 @@
         <v>5</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="AD1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="AF1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -7628,7 +7669,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -7732,7 +7773,7 @@
         <v>100</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -7836,7 +7877,7 @@
         <v>100</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L5" s="1">
         <v>1</v>
@@ -7940,7 +7981,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L6" s="1">
         <v>1</v>
@@ -8044,7 +8085,7 @@
         <v>100</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L7" s="1">
         <v>1</v>
@@ -8148,7 +8189,7 @@
         <v>100</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L8" s="1">
         <v>1</v>
@@ -8252,7 +8293,7 @@
         <v>100</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L9" s="1">
         <v>1</v>
@@ -8356,7 +8397,7 @@
         <v>100</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L10" s="1">
         <v>1</v>
@@ -8460,7 +8501,7 @@
         <v>100</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L11" s="1">
         <v>1</v>
@@ -8564,7 +8605,7 @@
         <v>100</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L12" s="1">
         <v>1</v>
@@ -8668,7 +8709,7 @@
         <v>100</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
@@ -8772,7 +8813,7 @@
         <v>100</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
@@ -8876,7 +8917,7 @@
         <v>100</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L15" s="1">
         <v>1</v>
@@ -8980,7 +9021,7 @@
         <v>100</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
@@ -9084,7 +9125,7 @@
         <v>100</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L17" s="1">
         <v>1</v>
@@ -9185,10 +9226,10 @@
         <v>6</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L18" s="1">
         <v>1</v>
@@ -9292,7 +9333,7 @@
         <v>100</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L19" s="1">
         <v>1</v>
@@ -9396,7 +9437,7 @@
         <v>100</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L20" s="1">
         <v>1</v>
@@ -9497,10 +9538,10 @@
         <v>9</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L21" s="1">
         <v>1</v>
@@ -9604,7 +9645,7 @@
         <v>100</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L22" s="1">
         <v>1</v>
@@ -9708,7 +9749,7 @@
         <v>100</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L23" s="1">
         <v>1</v>
@@ -9812,7 +9853,7 @@
         <v>100</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L24" s="1">
         <v>1</v>
@@ -9916,7 +9957,7 @@
         <v>100</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L25" s="1">
         <v>1</v>
@@ -10020,7 +10061,7 @@
         <v>100</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L26" s="1">
         <v>1</v>
@@ -10124,7 +10165,7 @@
         <v>100</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L27" s="1">
         <v>1</v>
@@ -10228,7 +10269,7 @@
         <v>100</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L28" s="1">
         <v>1</v>
@@ -10332,7 +10373,7 @@
         <v>100</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L29" s="1">
         <v>0</v>
@@ -10427,7 +10468,7 @@
         <v>28</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I30" s="1">
         <v>7</v>
@@ -10436,7 +10477,7 @@
         <v>100</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L30" s="1">
         <v>0</v>
@@ -10540,7 +10581,7 @@
         <v>100</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L31" s="1">
         <v>1</v>
@@ -10644,7 +10685,7 @@
         <v>100</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L32" s="1">
         <v>1</v>
@@ -10748,7 +10789,7 @@
         <v>100</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L33" s="1">
         <v>1</v>
@@ -10852,7 +10893,7 @@
         <v>100</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L34" s="1">
         <v>1</v>
@@ -10956,7 +10997,7 @@
         <v>100</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L35" s="1">
         <v>1</v>
@@ -11060,7 +11101,7 @@
         <v>100</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L36" s="1">
         <v>1</v>
@@ -11164,7 +11205,7 @@
         <v>100</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L37" s="1">
         <v>1</v>
@@ -11268,7 +11309,7 @@
         <v>100</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L38" s="1">
         <v>1</v>
@@ -11372,7 +11413,7 @@
         <v>100</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L39" s="1">
         <v>1</v>
@@ -11476,7 +11517,7 @@
         <v>100</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L40" s="1">
         <v>1</v>
@@ -11571,7 +11612,7 @@
         <v>39</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I41" s="1">
         <v>3</v>
@@ -11580,7 +11621,7 @@
         <v>100</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L41" s="1">
         <v>1</v>
@@ -11684,7 +11725,7 @@
         <v>100</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L42" s="1">
         <v>1</v>
@@ -11788,7 +11829,7 @@
         <v>100</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L43" s="1">
         <v>1</v>
@@ -11892,7 +11933,7 @@
         <v>100</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L44" s="1">
         <v>1</v>
@@ -11996,7 +12037,7 @@
         <v>100</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L45" s="1">
         <v>1</v>
@@ -12100,7 +12141,7 @@
         <v>100</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L46" s="1">
         <v>1</v>
@@ -12204,7 +12245,7 @@
         <v>100</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L47" s="1">
         <v>1</v>
@@ -12299,7 +12340,7 @@
         <v>46</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I48" s="1">
         <v>2</v>
@@ -12308,7 +12349,7 @@
         <v>100</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L48" s="1">
         <v>1</v>
@@ -12412,7 +12453,7 @@
         <v>100</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L49" s="1">
         <v>1</v>
@@ -12516,7 +12557,7 @@
         <v>100</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L50" s="1">
         <v>1</v>
@@ -12620,7 +12661,7 @@
         <v>100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L51" s="1">
         <v>1</v>
@@ -12724,7 +12765,7 @@
         <v>100</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L52" s="1">
         <v>1</v>
@@ -12828,7 +12869,7 @@
         <v>100</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L53" s="1">
         <v>1</v>
@@ -12932,7 +12973,7 @@
         <v>100</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L54" s="1">
         <v>0</v>
@@ -13027,7 +13068,7 @@
         <v>53</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I55" s="1">
         <v>9</v>
@@ -13036,7 +13077,7 @@
         <v>100</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L55" s="1">
         <v>0</v>
@@ -13140,7 +13181,7 @@
         <v>100</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L56" s="1">
         <v>1</v>
@@ -13244,7 +13285,7 @@
         <v>100</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L57" s="1">
         <v>1</v>
@@ -13348,7 +13389,7 @@
         <v>100</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L58" s="1">
         <v>1</v>
@@ -13452,7 +13493,7 @@
         <v>100</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L59" s="1">
         <v>1</v>
@@ -13556,7 +13597,7 @@
         <v>100</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L60" s="1">
         <v>1</v>
@@ -13660,7 +13701,7 @@
         <v>100</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L61" s="1">
         <v>1</v>
@@ -13764,7 +13805,7 @@
         <v>100</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L62" s="1">
         <v>1</v>
@@ -13868,7 +13909,7 @@
         <v>100</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L63" s="1">
         <v>1</v>
@@ -13972,7 +14013,7 @@
         <v>100</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L64" s="1">
         <v>1</v>
@@ -14076,7 +14117,7 @@
         <v>100</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L65" s="1">
         <v>1</v>
@@ -14180,7 +14221,7 @@
         <v>100</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L66" s="1">
         <v>1</v>
@@ -14284,7 +14325,7 @@
         <v>100</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L67" s="1">
         <v>1</v>
@@ -14388,7 +14429,7 @@
         <v>100</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L68" s="1">
         <v>1</v>
@@ -14492,7 +14533,7 @@
         <v>100</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L69" s="1">
         <v>1</v>
@@ -14596,7 +14637,7 @@
         <v>100</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L70" s="1">
         <v>1</v>
@@ -14700,7 +14741,7 @@
         <v>100</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L71" s="1">
         <v>1</v>
@@ -14804,7 +14845,7 @@
         <v>100</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L72" s="1">
         <v>1</v>
@@ -14908,7 +14949,7 @@
         <v>100</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L73" s="1">
         <v>1</v>
@@ -15012,7 +15053,7 @@
         <v>100</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L74" s="1">
         <v>1</v>
@@ -15116,7 +15157,7 @@
         <v>100</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L75" s="1">
         <v>1</v>
@@ -15220,7 +15261,7 @@
         <v>100</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L76" s="1">
         <v>1</v>
@@ -15324,7 +15365,7 @@
         <v>100</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L77" s="1">
         <v>1</v>
@@ -15428,7 +15469,7 @@
         <v>100</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L78" s="1">
         <v>1</v>
@@ -15532,7 +15573,7 @@
         <v>100</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L79" s="1">
         <v>1</v>
@@ -15636,7 +15677,7 @@
         <v>100</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L80" s="1">
         <v>1</v>
@@ -15740,7 +15781,7 @@
         <v>100</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L81" s="1">
         <v>1</v>
@@ -15844,7 +15885,7 @@
         <v>100</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L82" s="1">
         <v>1</v>
@@ -15948,7 +15989,7 @@
         <v>100</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L83" s="1">
         <v>1</v>
@@ -16052,7 +16093,7 @@
         <v>100</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L84" s="1">
         <v>1</v>
@@ -16156,7 +16197,7 @@
         <v>100</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L85" s="1">
         <v>1</v>
@@ -16243,7 +16284,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -16252,13 +16293,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -16292,13 +16333,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -16315,13 +16356,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -16338,13 +16379,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -16361,13 +16402,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -16384,13 +16425,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -16407,13 +16448,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -16450,13 +16491,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -16465,16 +16506,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -16522,13 +16563,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G3" s="1">
         <v>12</v>
@@ -16555,13 +16596,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G4" s="1">
         <v>12</v>
@@ -16588,13 +16629,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G5" s="1">
         <v>12</v>
@@ -16621,13 +16662,13 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G6" s="1">
         <v>12</v>
@@ -16654,13 +16695,13 @@
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G7" s="1">
         <v>12</v>
@@ -16690,10 +16731,10 @@
         <v>124</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G8" s="1">
         <v>12</v>
@@ -16720,13 +16761,13 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>216</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="1">
         <v>12</v>
@@ -16753,13 +16794,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>219</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G10" s="1">
         <v>12</v>
@@ -16786,13 +16827,13 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G11" s="1">
         <v>12</v>
@@ -16819,13 +16860,13 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G12" s="1">
         <v>12</v>
@@ -16852,13 +16893,13 @@
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G13" s="1">
         <v>12</v>
@@ -16885,13 +16926,13 @@
         <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G14" s="1">
         <v>12</v>
@@ -16918,13 +16959,13 @@
         <v>4</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G15" s="1">
         <v>12</v>
@@ -16951,13 +16992,13 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G16" s="1">
         <v>12</v>
@@ -16984,13 +17025,13 @@
         <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G17" s="1">
         <v>12</v>
@@ -17017,13 +17058,13 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>235</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G18" s="1">
         <v>12</v>
@@ -17050,13 +17091,13 @@
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G19" s="1">
         <v>12</v>
@@ -17110,16 +17151,16 @@
         <v>99</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Added the basic validations.
</commit_message>
<xml_diff>
--- a/Common/DataSchema/Schema.xlsx
+++ b/Common/DataSchema/Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMaestroRamirez\source\repos\DanielMaestro\Alessa\Common\DataSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A8D2BC-7F8A-4515-81DA-8E1FE7C688C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEB91F-A51F-440E-92C6-20CB1DC2E6C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Alessa.TableConfiguration" sheetId="18" r:id="rId1"/>
@@ -31,7 +31,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Alessa.FieldDefinition!$A$1:$I$85</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Alessa.FieldDefinitionUi!$A$1:$AF$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Alessa.FieldDefinitionUi!$A$1:$AJ$85</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Alessa.FieldKeysRelationship!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Alessa.TableDefinition!$A$1:$E$1</definedName>
   </definedNames>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="330">
   <si>
     <t>ItemName</t>
   </si>
@@ -1104,6 +1104,18 @@
   </si>
   <si>
     <t>From(Samples.HideEnableSample) Select(25 AS HideWhen2OrMore, 'Record {{HideEnableSampleId}}' AS EnableWhen5) Limit(1)</t>
+  </si>
+  <si>
+    <t>FormatErrorMsg</t>
+  </si>
+  <si>
+    <t>RangeMin</t>
+  </si>
+  <si>
+    <t>RangeMax</t>
+  </si>
+  <si>
+    <t>RangeErrorMsg</t>
   </si>
 </sst>
 </file>
@@ -4724,7 +4736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB104D6-C294-4D4F-9258-F7A2971580B6}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -7420,12 +7432,12 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BCF39D-315F-4810-8B54-5D5D18B35E09}">
-  <dimension ref="A1:AF85"/>
+  <dimension ref="A1:AJ85"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7445,10 +7457,10 @@
     <col min="20" max="21" width="7.28515625" style="1" customWidth="1"/>
     <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="6.42578125" customWidth="1"/>
-    <col min="24" max="28" width="6.5703125" customWidth="1"/>
+    <col min="24" max="32" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>102</v>
       </c>
@@ -7522,31 +7534,43 @@
         <v>159</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -7622,16 +7646,28 @@
         <v>18</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f>VLOOKUP($G3,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7649,11 +7685,11 @@
         <v>Integer</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF3,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ3,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F3" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF3,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ3,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G3" s="1">
@@ -7734,8 +7770,20 @@
       <c r="AF3" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>VLOOKUP($G4,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7753,11 +7801,11 @@
         <v>Text</v>
       </c>
       <c r="E4" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF4,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ4,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F4" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF4,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ4,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G4" s="1">
@@ -7838,8 +7886,20 @@
       <c r="AF4" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>VLOOKUP($G5,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7857,11 +7917,11 @@
         <v>Text</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF5,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ5,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F5" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF5,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ5,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G5" s="1">
@@ -7942,8 +8002,20 @@
       <c r="AF5" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>VLOOKUP($G6,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>1</v>
@@ -7961,11 +8033,11 @@
         <v>Bit</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF6,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ6,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F6" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF6,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ6,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G6" s="1">
@@ -8046,8 +8118,20 @@
       <c r="AF6" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f>VLOOKUP($G7,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8065,11 +8149,11 @@
         <v>Integer</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF7,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ7,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F7" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF7,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ7,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G7" s="1">
@@ -8150,8 +8234,20 @@
       <c r="AF7" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f>VLOOKUP($G8,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8169,11 +8265,11 @@
         <v>Bit</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF8,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ8,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F8" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF8,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ8,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G8" s="1">
@@ -8254,8 +8350,20 @@
       <c r="AF8" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>VLOOKUP($G9,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8273,11 +8381,11 @@
         <v>Integer</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF9,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ9,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F9" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF9,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ9,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G9" s="1">
@@ -8358,8 +8466,20 @@
       <c r="AF9" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>VLOOKUP($G10,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8377,11 +8497,11 @@
         <v>Text</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF10,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ10,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F10" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF10,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ10,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G10" s="1">
@@ -8462,8 +8582,20 @@
       <c r="AF10" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f>VLOOKUP($G11,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8481,11 +8613,11 @@
         <v>Text</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF11,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ11,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F11" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF11,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ11,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G11" s="1">
@@ -8566,8 +8698,20 @@
       <c r="AF11" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI11" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>VLOOKUP($G12,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>2</v>
@@ -8585,11 +8729,11 @@
         <v>Bit</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF12,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ12,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F12" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF12,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ12,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G12" s="1">
@@ -8670,8 +8814,20 @@
       <c r="AF12" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>VLOOKUP($G13,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8689,11 +8845,11 @@
         <v>Text</v>
       </c>
       <c r="E13" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF13,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ13,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF13,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ13,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G13" s="1">
@@ -8765,17 +8921,29 @@
       <c r="AC13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="1">
+      <c r="AD13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="1">
         <v>12</v>
       </c>
-      <c r="AF13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AJ13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f>VLOOKUP($G14,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8793,11 +8961,11 @@
         <v>Bit</v>
       </c>
       <c r="E14" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF14,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ14,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF14,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ14,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G14" s="1">
@@ -8869,17 +9037,29 @@
       <c r="AC14" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="1">
+      <c r="AD14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI14" s="1">
         <v>12</v>
       </c>
-      <c r="AF14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AJ14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>VLOOKUP($G15,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -8897,11 +9077,11 @@
         <v>Date</v>
       </c>
       <c r="E15" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF15,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ15,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF15,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ15,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G15" s="1">
@@ -8973,17 +9153,29 @@
       <c r="AC15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD15" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="1">
+      <c r="AD15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="1">
         <v>12</v>
       </c>
-      <c r="AF15" s="1">
+      <c r="AJ15" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f>VLOOKUP($G16,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9001,11 +9193,11 @@
         <v>DateTime</v>
       </c>
       <c r="E16" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF16,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ16,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF16,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ16,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G16" s="1">
@@ -9077,17 +9269,29 @@
       <c r="AC16" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE16" s="1">
+      <c r="AD16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI16" s="1">
         <v>12</v>
       </c>
-      <c r="AF16" s="1">
+      <c r="AJ16" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>VLOOKUP($G17,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9105,11 +9309,11 @@
         <v>Decimal</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF17,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ17,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF17,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ17,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G17" s="1">
@@ -9181,17 +9385,29 @@
       <c r="AC17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD17" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE17" s="1">
+      <c r="AD17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="1">
         <v>12</v>
       </c>
-      <c r="AF17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AJ17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f>VLOOKUP($G18,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9209,11 +9425,11 @@
         <v>Integer</v>
       </c>
       <c r="E18" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF18,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ18,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F18" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF18,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ18,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G18" s="1">
@@ -9285,17 +9501,29 @@
       <c r="AC18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE18" s="1">
+      <c r="AD18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="1">
         <v>12</v>
       </c>
-      <c r="AF18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AJ18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f>VLOOKUP($G19,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9313,11 +9541,11 @@
         <v>Decimal</v>
       </c>
       <c r="E19" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF19,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ19,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F19" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF19,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ19,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>NumericTab</v>
       </c>
       <c r="G19" s="1">
@@ -9389,17 +9617,29 @@
       <c r="AC19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD19" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="1">
+      <c r="AD19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="1">
         <v>12</v>
       </c>
-      <c r="AF19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AJ19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f>VLOOKUP($G20,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9417,11 +9657,11 @@
         <v>RichText</v>
       </c>
       <c r="E20" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF20,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ20,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F20" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF20,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ20,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G20" s="1">
@@ -9493,17 +9733,29 @@
       <c r="AC20" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE20" s="1">
+      <c r="AD20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI20" s="1">
         <v>12</v>
       </c>
-      <c r="AF20" s="1">
+      <c r="AJ20" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f>VLOOKUP($G21,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9521,11 +9773,11 @@
         <v>Text</v>
       </c>
       <c r="E21" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF21,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ21,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF21,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ21,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G21" s="1">
@@ -9597,17 +9849,29 @@
       <c r="AC21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="1">
+      <c r="AD21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="1">
         <v>12</v>
       </c>
-      <c r="AF21" s="1">
+      <c r="AJ21" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f>VLOOKUP($G22,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9625,11 +9889,11 @@
         <v>TextArea</v>
       </c>
       <c r="E22" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF22,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ22,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F22" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF22,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ22,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>TextTab</v>
       </c>
       <c r="G22" s="1">
@@ -9701,17 +9965,29 @@
       <c r="AC22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD22" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE22" s="1">
+      <c r="AD22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI22" s="1">
         <v>12</v>
       </c>
-      <c r="AF22" s="1">
+      <c r="AJ22" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f>VLOOKUP($G23,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>3</v>
@@ -9729,11 +10005,11 @@
         <v>Time</v>
       </c>
       <c r="E23" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF23,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ23,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>BasicColumnGroup</v>
       </c>
       <c r="F23" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF23,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ23,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>DateTab</v>
       </c>
       <c r="G23" s="1">
@@ -9805,17 +10081,29 @@
       <c r="AC23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE23" s="1">
+      <c r="AD23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="1">
         <v>12</v>
       </c>
-      <c r="AF23" s="1">
+      <c r="AJ23" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f>VLOOKUP($G24,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9833,11 +10121,11 @@
         <v>Integer</v>
       </c>
       <c r="E24" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF24,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ24,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F24" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF24,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ24,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G24" s="1">
@@ -9918,8 +10206,20 @@
       <c r="AF24" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f>VLOOKUP($G25,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -9937,11 +10237,11 @@
         <v>Text</v>
       </c>
       <c r="E25" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF25,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ25,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F25" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF25,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ25,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G25" s="1">
@@ -10022,8 +10322,20 @@
       <c r="AF25" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f>VLOOKUP($G26,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10041,11 +10353,11 @@
         <v>DateTime</v>
       </c>
       <c r="E26" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF26,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ26,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF26,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ26,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G26" s="1">
@@ -10126,8 +10438,20 @@
       <c r="AF26" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>VLOOKUP($G27,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10145,11 +10469,11 @@
         <v>Integer</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF27,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ27,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F27" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF27,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ27,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G27" s="1">
@@ -10230,8 +10554,20 @@
       <c r="AF27" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f>VLOOKUP($G28,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10249,11 +10585,11 @@
         <v>Integer</v>
       </c>
       <c r="E28" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF28,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ28,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F28" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF28,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ28,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G28" s="1">
@@ -10334,8 +10670,20 @@
       <c r="AF28" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ28" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f>VLOOKUP($G29,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10353,11 +10701,11 @@
         <v>Bit</v>
       </c>
       <c r="E29" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF29,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ29,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F29" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF29,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ29,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G29" s="1">
@@ -10438,8 +10786,20 @@
       <c r="AF29" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f>VLOOKUP($G30,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>4</v>
@@ -10457,11 +10817,11 @@
         <v>Bit</v>
       </c>
       <c r="E30" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF30,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ30,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F30" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF30,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ30,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G30" s="1">
@@ -10542,8 +10902,20 @@
       <c r="AF30" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ30" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>VLOOKUP($G31,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10561,11 +10933,11 @@
         <v>SingleSelect</v>
       </c>
       <c r="E31" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF31,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ31,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF31,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ31,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>List</v>
       </c>
       <c r="G31" s="1">
@@ -10637,17 +11009,29 @@
       <c r="AC31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="1">
+      <c r="AD31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI31" s="1">
         <v>12</v>
       </c>
-      <c r="AF31" s="1">
+      <c r="AJ31" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>VLOOKUP($G32,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10665,11 +11049,11 @@
         <v>Text</v>
       </c>
       <c r="E32" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF32,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ32,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF32,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ32,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G32" s="1">
@@ -10741,17 +11125,29 @@
       <c r="AC32" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD32" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE32" s="1">
+      <c r="AD32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI32" s="1">
         <v>12</v>
       </c>
-      <c r="AF32" s="1">
+      <c r="AJ32" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f>VLOOKUP($G33,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10769,11 +11165,11 @@
         <v>DateTime</v>
       </c>
       <c r="E33" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF33,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ33,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF33,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ33,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G33" s="1">
@@ -10845,17 +11241,29 @@
       <c r="AC33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="1">
+      <c r="AD33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="1">
         <v>12</v>
       </c>
-      <c r="AF33" s="1">
+      <c r="AJ33" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>VLOOKUP($G34,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10873,11 +11281,11 @@
         <v>Integer</v>
       </c>
       <c r="E34" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF34,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ34,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF34,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ34,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G34" s="1">
@@ -10949,17 +11357,29 @@
       <c r="AC34" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="1">
+      <c r="AD34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI34" s="1">
         <v>12</v>
       </c>
-      <c r="AF34" s="1">
+      <c r="AJ34" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f>VLOOKUP($G35,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>5</v>
@@ -10977,11 +11397,11 @@
         <v>Radio</v>
       </c>
       <c r="E35" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF35,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ35,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>CatalogsJoinSampleViewGroup</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF35,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ35,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Radio</v>
       </c>
       <c r="G35" s="1">
@@ -11053,17 +11473,29 @@
       <c r="AC35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD35" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="1">
+      <c r="AD35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI35" s="1">
         <v>12</v>
       </c>
-      <c r="AF35" s="1">
+      <c r="AJ35" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f>VLOOKUP($G36,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -11081,11 +11513,11 @@
         <v>Integer</v>
       </c>
       <c r="E36" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF36,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ36,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F36" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF36,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ36,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G36" s="1">
@@ -11166,8 +11598,20 @@
       <c r="AF36" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f>VLOOKUP($G37,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -11185,11 +11629,11 @@
         <v>Bit</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF37,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ37,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F37" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF37,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ37,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G37" s="1">
@@ -11270,8 +11714,20 @@
       <c r="AF37" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ37" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f>VLOOKUP($G38,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>6</v>
@@ -11289,11 +11745,11 @@
         <v>Text</v>
       </c>
       <c r="E38" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF38,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ38,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF38,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ38,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G38" s="1">
@@ -11374,8 +11830,20 @@
       <c r="AF38" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ38" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f>VLOOKUP($G39,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11393,11 +11861,11 @@
         <v>Bit</v>
       </c>
       <c r="E39" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF39,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ39,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F39" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF39,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ39,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G39" s="1">
@@ -11469,17 +11937,29 @@
       <c r="AC39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD39" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE39" s="1">
+      <c r="AD39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI39" s="1">
         <v>12</v>
       </c>
-      <c r="AF39" s="1">
+      <c r="AJ39" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f>VLOOKUP($G40,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11497,11 +11977,11 @@
         <v>Text</v>
       </c>
       <c r="E40" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF40,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ40,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF40,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ40,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G40" s="1">
@@ -11573,17 +12053,29 @@
       <c r="AC40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE40" s="1">
+      <c r="AD40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI40" s="1">
         <v>12</v>
       </c>
-      <c r="AF40" s="1">
+      <c r="AJ40" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f>VLOOKUP($G41,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11601,11 +12093,11 @@
         <v>Decimal</v>
       </c>
       <c r="E41" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF41,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ41,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF41,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ41,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G41" s="1">
@@ -11677,17 +12169,29 @@
       <c r="AC41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE41" s="1">
+      <c r="AD41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI41" s="1">
         <v>12</v>
       </c>
-      <c r="AF41" s="1">
+      <c r="AJ41" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f>VLOOKUP($G42,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11705,11 +12209,11 @@
         <v>Text</v>
       </c>
       <c r="E42" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF42,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ42,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF42,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ42,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Furthermore</v>
       </c>
       <c r="G42" s="1">
@@ -11781,17 +12285,29 @@
       <c r="AC42" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE42" s="1">
+      <c r="AD42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI42" s="1">
         <v>12</v>
       </c>
-      <c r="AF42" s="1">
+      <c r="AJ42" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f>VLOOKUP($G43,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11809,11 +12325,11 @@
         <v>MultiselectList</v>
       </c>
       <c r="E43" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF43,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ43,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF43,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ43,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>SelectHide</v>
       </c>
       <c r="G43" s="1">
@@ -11885,17 +12401,29 @@
       <c r="AC43" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE43" s="1">
+      <c r="AD43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI43" s="1">
         <v>12</v>
       </c>
-      <c r="AF43" s="1">
+      <c r="AJ43" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f>VLOOKUP($G44,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -11913,11 +12441,11 @@
         <v>Text</v>
       </c>
       <c r="E44" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF44,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ44,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF44,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ44,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G44" s="1">
@@ -11989,17 +12517,29 @@
       <c r="AC44" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE44" s="1">
+      <c r="AD44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH44" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI44" s="1">
         <v>12</v>
       </c>
-      <c r="AF44" s="1">
+      <c r="AJ44" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f>VLOOKUP($G45,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -12017,11 +12557,11 @@
         <v>Text</v>
       </c>
       <c r="E45" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF45,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ45,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF45,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ45,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Furthermore</v>
       </c>
       <c r="G45" s="1">
@@ -12093,17 +12633,29 @@
       <c r="AC45" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE45" s="1">
+      <c r="AD45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH45" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI45" s="1">
         <v>12</v>
       </c>
-      <c r="AF45" s="1">
+      <c r="AJ45" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f>VLOOKUP($G46,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>7</v>
@@ -12121,11 +12673,11 @@
         <v>Text</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF46,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ46,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>HideEnableSampleViewGroup</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF46,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ46,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CheckboxHide</v>
       </c>
       <c r="G46" s="1">
@@ -12197,17 +12749,29 @@
       <c r="AC46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD46" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE46" s="1">
+      <c r="AD46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH46" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI46" s="1">
         <v>12</v>
       </c>
-      <c r="AF46" s="1">
+      <c r="AJ46" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f>VLOOKUP($G47,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12225,11 +12789,11 @@
         <v>Bit</v>
       </c>
       <c r="E47" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF47,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ47,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF47,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ47,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G47" s="1">
@@ -12310,8 +12874,20 @@
       <c r="AF47" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI47" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ47" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>VLOOKUP($G48,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12329,11 +12905,11 @@
         <v>Text</v>
       </c>
       <c r="E48" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF48,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ48,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF48,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ48,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G48" s="1">
@@ -12414,8 +12990,20 @@
       <c r="AF48" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI48" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f>VLOOKUP($G49,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12433,11 +13021,11 @@
         <v>Integer</v>
       </c>
       <c r="E49" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF49,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ49,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF49,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ49,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G49" s="1">
@@ -12518,8 +13106,20 @@
       <c r="AF49" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI49" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ49" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f>VLOOKUP($G50,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12537,11 +13137,11 @@
         <v>Decimal</v>
       </c>
       <c r="E50" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF50,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ50,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF50,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ50,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G50" s="1">
@@ -12622,8 +13222,20 @@
       <c r="AF50" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ50" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f>VLOOKUP($G51,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12641,11 +13253,11 @@
         <v>Text</v>
       </c>
       <c r="E51" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF51,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ51,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF51,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ51,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G51" s="1">
@@ -12726,8 +13338,20 @@
       <c r="AF51" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ51" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f>VLOOKUP($G52,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12745,11 +13369,11 @@
         <v>Text</v>
       </c>
       <c r="E52" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF52,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ52,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F52" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF52,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ52,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G52" s="1">
@@ -12830,8 +13454,20 @@
       <c r="AF52" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ52" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f>VLOOKUP($G53,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12849,11 +13485,11 @@
         <v>Text</v>
       </c>
       <c r="E53" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF53,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ53,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F53" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF53,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ53,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G53" s="1">
@@ -12934,8 +13570,20 @@
       <c r="AF53" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ53" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f>VLOOKUP($G54,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -12953,11 +13601,11 @@
         <v>Bit</v>
       </c>
       <c r="E54" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF54,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ54,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F54" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF54,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ54,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G54" s="1">
@@ -13038,8 +13686,20 @@
       <c r="AF54" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ54" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f>VLOOKUP($G55,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>8</v>
@@ -13057,11 +13717,11 @@
         <v>Bit</v>
       </c>
       <c r="E55" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF55,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ55,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F55" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF55,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ55,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G55" s="1">
@@ -13142,8 +13802,20 @@
       <c r="AF55" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI55" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ55" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f>VLOOKUP($G56,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -13161,11 +13833,11 @@
         <v>Integer</v>
       </c>
       <c r="E56" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF56,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ56,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F56" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF56,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ56,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G56" s="1">
@@ -13246,8 +13918,20 @@
       <c r="AF56" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ56" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f>VLOOKUP($G57,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -13265,11 +13949,11 @@
         <v>Bit</v>
       </c>
       <c r="E57" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF57,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ57,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F57" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF57,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ57,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G57" s="1">
@@ -13350,8 +14034,20 @@
       <c r="AF57" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI57" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ57" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f>VLOOKUP($G58,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>9</v>
@@ -13369,11 +14065,11 @@
         <v>Integer</v>
       </c>
       <c r="E58" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF58,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ58,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F58" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF58,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ58,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G58" s="1">
@@ -13454,8 +14150,20 @@
       <c r="AF58" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ58" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f>VLOOKUP($G59,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -13473,11 +14181,11 @@
         <v>Integer</v>
       </c>
       <c r="E59" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF59,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ59,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F59" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF59,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ59,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G59" s="1">
@@ -13558,8 +14266,20 @@
       <c r="AF59" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI59" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ59" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f>VLOOKUP($G60,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -13577,11 +14297,11 @@
         <v>Bit</v>
       </c>
       <c r="E60" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF60,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ60,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F60" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF60,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ60,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G60" s="1">
@@ -13662,8 +14382,20 @@
       <c r="AF60" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI60" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ60" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f>VLOOKUP($G61,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>10</v>
@@ -13681,11 +14413,11 @@
         <v>Integer</v>
       </c>
       <c r="E61" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF61,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ61,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F61" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF61,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ61,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G61" s="1">
@@ -13766,8 +14498,20 @@
       <c r="AF61" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI61" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ61" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f>VLOOKUP($G62,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>11</v>
@@ -13785,11 +14529,11 @@
         <v>DateTime</v>
       </c>
       <c r="E62" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF62,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ62,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F62" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF62,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ62,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G62" s="1">
@@ -13870,8 +14614,20 @@
       <c r="AF62" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI62" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ62" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>VLOOKUP($G63,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>11</v>
@@ -13889,11 +14645,11 @@
         <v>Integer</v>
       </c>
       <c r="E63" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF63,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ63,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F63" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF63,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ63,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G63" s="1">
@@ -13974,8 +14730,20 @@
       <c r="AF63" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f>VLOOKUP($G64,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -13993,11 +14761,11 @@
         <v>MultiselectCheckbox</v>
       </c>
       <c r="E64" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF64,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ64,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F64" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF64,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ64,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>MultiCheckbox</v>
       </c>
       <c r="G64" s="1">
@@ -14069,17 +14837,29 @@
       <c r="AC64" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD64" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE64" s="1">
+      <c r="AD64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG64" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH64" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI64" s="1">
         <v>12</v>
       </c>
-      <c r="AF64" s="1">
+      <c r="AJ64" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f>VLOOKUP($G65,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -14097,11 +14877,11 @@
         <v>DateTime</v>
       </c>
       <c r="E65" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF65,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ65,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F65" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF65,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ65,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CommonData</v>
       </c>
       <c r="G65" s="1">
@@ -14173,17 +14953,29 @@
       <c r="AC65" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD65" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE65" s="1">
+      <c r="AD65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG65" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH65" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI65" s="1">
         <v>12</v>
       </c>
-      <c r="AF65" s="1">
+      <c r="AJ65" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f>VLOOKUP($G66,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -14201,11 +14993,11 @@
         <v>MultiselectList</v>
       </c>
       <c r="E66" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF66,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ66,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F66" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF66,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ66,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>MultiSelect</v>
       </c>
       <c r="G66" s="1">
@@ -14277,17 +15069,29 @@
       <c r="AC66" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD66" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE66" s="1">
+      <c r="AD66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG66" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH66" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI66" s="1">
         <v>12</v>
       </c>
-      <c r="AF66" s="1">
+      <c r="AJ66" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f>VLOOKUP($G67,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -14305,11 +15109,11 @@
         <v>Integer</v>
       </c>
       <c r="E67" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF67,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ67,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F67" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF67,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ67,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CommonData</v>
       </c>
       <c r="G67" s="1">
@@ -14381,17 +15185,29 @@
       <c r="AC67" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD67" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE67" s="1">
+      <c r="AD67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG67" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH67" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI67" s="1">
         <v>12</v>
       </c>
-      <c r="AF67" s="1">
+      <c r="AJ67" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f>VLOOKUP($G68,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>12</v>
@@ -14409,11 +15225,11 @@
         <v>TableReference</v>
       </c>
       <c r="E68" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF68,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ68,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>MultiSelectSampleViewGroup</v>
       </c>
       <c r="F68" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF68,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ68,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Grid</v>
       </c>
       <c r="G68" s="1">
@@ -14485,17 +15301,29 @@
       <c r="AC68" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD68" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE68" s="1">
+      <c r="AD68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG68" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH68" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI68" s="1">
         <v>12</v>
       </c>
-      <c r="AF68" s="1">
+      <c r="AJ68" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f>VLOOKUP($G69,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -14513,11 +15341,11 @@
         <v>Text</v>
       </c>
       <c r="E69" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF69,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ69,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F69" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF69,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ69,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G69" s="1">
@@ -14598,8 +15426,20 @@
       <c r="AF69" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI69" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ69" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f>VLOOKUP($G70,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -14617,11 +15457,11 @@
         <v>Bit</v>
       </c>
       <c r="E70" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF70,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ70,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F70" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF70,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ70,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G70" s="1">
@@ -14702,8 +15542,20 @@
       <c r="AF70" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI70" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ70" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f>VLOOKUP($G71,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>13</v>
@@ -14721,11 +15573,11 @@
         <v>Integer</v>
       </c>
       <c r="E71" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF71,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ71,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v/>
       </c>
       <c r="F71" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF71,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ71,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v/>
       </c>
       <c r="G71" s="1">
@@ -14806,8 +15658,20 @@
       <c r="AF71" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AJ71" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f>VLOOKUP($G72,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14825,11 +15689,11 @@
         <v>Integer</v>
       </c>
       <c r="E72" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF72,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ72,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F72" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF72,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ72,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G72" s="1">
@@ -14901,17 +15765,29 @@
       <c r="AC72" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD72" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE72" s="1">
+      <c r="AD72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG72" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH72" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI72" s="1">
         <v>12</v>
       </c>
-      <c r="AF72" s="1">
+      <c r="AJ72" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f>VLOOKUP($G73,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -14929,11 +15805,11 @@
         <v>DateTime</v>
       </c>
       <c r="E73" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF73,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ73,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F73" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF73,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ73,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G73" s="1">
@@ -15005,17 +15881,29 @@
       <c r="AC73" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD73" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE73" s="1">
+      <c r="AD73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG73" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH73" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI73" s="1">
         <v>12</v>
       </c>
-      <c r="AF73" s="1">
+      <c r="AJ73" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f>VLOOKUP($G74,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15033,11 +15921,11 @@
         <v>Integer</v>
       </c>
       <c r="E74" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF74,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ74,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F74" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF74,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ74,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G74" s="1">
@@ -15109,17 +15997,29 @@
       <c r="AC74" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD74" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE74" s="1">
+      <c r="AD74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG74" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH74" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI74" s="1">
         <v>12</v>
       </c>
-      <c r="AF74" s="1">
+      <c r="AJ74" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f>VLOOKUP($G75,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15137,11 +16037,11 @@
         <v>Integer</v>
       </c>
       <c r="E75" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF75,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ75,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F75" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF75,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ75,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G75" s="1">
@@ -15213,17 +16113,29 @@
       <c r="AC75" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD75" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE75" s="1">
+      <c r="AD75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG75" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH75" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI75" s="1">
         <v>12</v>
       </c>
-      <c r="AF75" s="1">
+      <c r="AJ75" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f>VLOOKUP($G76,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15241,11 +16153,11 @@
         <v>Text</v>
       </c>
       <c r="E76" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF76,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ76,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F76" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF76,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ76,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G76" s="1">
@@ -15317,17 +16229,29 @@
       <c r="AC76" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD76" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE76" s="1">
+      <c r="AD76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG76" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH76" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI76" s="1">
         <v>12</v>
       </c>
-      <c r="AF76" s="1">
+      <c r="AJ76" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>VLOOKUP($G77,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15345,11 +16269,11 @@
         <v>Text</v>
       </c>
       <c r="E77" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF77,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ77,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F77" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF77,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ77,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G77" s="1">
@@ -15421,17 +16345,29 @@
       <c r="AC77" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD77" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE77" s="1">
+      <c r="AD77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG77" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH77" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI77" s="1">
         <v>12</v>
       </c>
-      <c r="AF77" s="1">
+      <c r="AJ77" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f>VLOOKUP($G78,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15449,11 +16385,11 @@
         <v>DateTime</v>
       </c>
       <c r="E78" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF78,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ78,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F78" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF78,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ78,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Advanced</v>
       </c>
       <c r="G78" s="1">
@@ -15525,17 +16461,29 @@
       <c r="AC78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD78" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE78" s="1">
+      <c r="AD78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG78" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH78" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI78" s="1">
         <v>12</v>
       </c>
-      <c r="AF78" s="1">
+      <c r="AJ78" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f>VLOOKUP($G79,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15553,11 +16501,11 @@
         <v>Text</v>
       </c>
       <c r="E79" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF79,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ79,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F79" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF79,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ79,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G79" s="1">
@@ -15629,17 +16577,29 @@
       <c r="AC79" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD79" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE79" s="1">
+      <c r="AD79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG79" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH79" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI79" s="1">
         <v>12</v>
       </c>
-      <c r="AF79" s="1">
+      <c r="AJ79" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f>VLOOKUP($G80,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>14</v>
@@ -15657,11 +16617,11 @@
         <v>Text</v>
       </c>
       <c r="E80" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF80,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ80,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ValidationGroup</v>
       </c>
       <c r="F80" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF80,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ80,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Basic</v>
       </c>
       <c r="G80" s="1">
@@ -15733,17 +16693,29 @@
       <c r="AC80" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD80" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE80" s="1">
+      <c r="AD80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH80" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI80" s="1">
         <v>12</v>
       </c>
-      <c r="AF80" s="1">
+      <c r="AJ80" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f>VLOOKUP($G81,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -15761,11 +16733,11 @@
         <v>Integer</v>
       </c>
       <c r="E81" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF81,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ81,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F81" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF81,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ81,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G81" s="1">
@@ -15837,17 +16809,29 @@
       <c r="AC81" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD81" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE81" s="1">
+      <c r="AD81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG81" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH81" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI81" s="1">
         <v>12</v>
       </c>
-      <c r="AF81" s="1">
+      <c r="AJ81" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f>VLOOKUP($G82,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -15865,11 +16849,11 @@
         <v>Text</v>
       </c>
       <c r="E82" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF82,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ82,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F82" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF82,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ82,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G82" s="1">
@@ -15941,17 +16925,29 @@
       <c r="AC82" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD82" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE82" s="1">
+      <c r="AD82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG82" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH82" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI82" s="1">
         <v>12</v>
       </c>
-      <c r="AF82" s="1">
+      <c r="AJ82" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f>VLOOKUP($G83,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -15969,11 +16965,11 @@
         <v>Text</v>
       </c>
       <c r="E83" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF83,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ83,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F83" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF83,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ83,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G83" s="1">
@@ -16045,17 +17041,29 @@
       <c r="AC83" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD83" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE83" s="1">
+      <c r="AD83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG83" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH83" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI83" s="1">
         <v>12</v>
       </c>
-      <c r="AF83" s="1">
+      <c r="AJ83" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f>VLOOKUP($G84,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -16073,11 +17081,11 @@
         <v>Bit</v>
       </c>
       <c r="E84" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF84,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ84,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F84" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF84,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ84,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>Form</v>
       </c>
       <c r="G84" s="1">
@@ -16149,17 +17157,29 @@
       <c r="AC84" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD84" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE84" s="1">
+      <c r="AD84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG84" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH84" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI84" s="1">
         <v>12</v>
       </c>
-      <c r="AF84" s="1">
+      <c r="AJ84" s="1">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f>VLOOKUP($G85,Alessa.FieldDefinition!$A$3:$I$85,3)</f>
         <v>15</v>
@@ -16177,11 +17197,11 @@
         <v>TableReference</v>
       </c>
       <c r="E85" s="1" t="str">
-        <f>IFERROR( VLOOKUP($AF85,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
+        <f>IFERROR( VLOOKUP($AJ85,Alessa.FieldGroupDetail!$A$3:$O$105,2), "")</f>
         <v>ALexTableGroup</v>
       </c>
       <c r="F85" s="1" t="str">
-        <f>IFERROR(VLOOKUP($AF85,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
+        <f>IFERROR(VLOOKUP($AJ85,Alessa.FieldGroupDetail!$A$3:$O$105,4), "")</f>
         <v>CatalogTypes</v>
       </c>
       <c r="G85" s="1">
@@ -16253,18 +17273,30 @@
       <c r="AC85" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AD85" s="1">
-        <v>1</v>
-      </c>
-      <c r="AE85" s="1">
+      <c r="AD85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG85" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH85" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI85" s="1">
         <v>12</v>
       </c>
-      <c r="AF85" s="1">
+      <c r="AJ85" s="1">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AF85" xr:uid="{98088FFF-07F4-4BB5-BAC5-BF377CA38131}"/>
+  <autoFilter ref="A1:AJ85" xr:uid="{98088FFF-07F4-4BB5-BAC5-BF377CA38131}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Just making some improvements to the basic validations
</commit_message>
<xml_diff>
--- a/Common/DataSchema/Schema.xlsx
+++ b/Common/DataSchema/Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielMaestroRamirez\source\repos\DanielMaestro\Alessa\Common\DataSchema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FEB91F-A51F-440E-92C6-20CB1DC2E6C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23205C29-6D7D-4188-A04A-800DBEA0EB40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{CD000836-11FC-47AB-934E-5C244566BA80}"/>
   </bookViews>
   <sheets>
     <sheet name="Alessa.TableConfiguration" sheetId="18" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="333">
   <si>
     <t>ItemName</t>
   </si>
@@ -1116,6 +1116,15 @@
   </si>
   <si>
     <t>RangeErrorMsg</t>
+  </si>
+  <si>
+    <t>Type any number but 5.</t>
+  </si>
+  <si>
+    <t>Only accepst number 5</t>
+  </si>
+  <si>
+    <t>^\w+([-+.']\w+)*@\w+([-.]\w+)*\.\w+([-.]\w+)*$</t>
   </si>
 </sst>
 </file>
@@ -3535,7 +3544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4862,8 +4871,8 @@
   <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D72" sqref="D72:D80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7434,10 +7443,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1BCF39D-315F-4810-8B54-5D5D18B35E09}">
   <dimension ref="A1:AJ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomLeft" activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15706,7 +15715,7 @@
         <v>1</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>100</v>
+        <v>330</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>184</v>
@@ -15938,7 +15947,7 @@
         <v>3</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>100</v>
+        <v>331</v>
       </c>
       <c r="K74" s="1" t="s">
         <v>184</v>
@@ -16098,11 +16107,11 @@
       <c r="X75" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Y75" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z75" s="1" t="s">
-        <v>100</v>
+      <c r="Y75" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z75" s="1">
+        <v>10</v>
       </c>
       <c r="AA75" s="1" t="s">
         <v>100</v>
@@ -16206,7 +16215,7 @@
         <v>0</v>
       </c>
       <c r="V76" s="1" t="s">
-        <v>100</v>
+        <v>332</v>
       </c>
       <c r="W76" s="1" t="s">
         <v>100</v>
@@ -16672,11 +16681,11 @@
       <c r="V80" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="W80" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="X80" s="1" t="s">
-        <v>100</v>
+      <c r="W80" s="1">
+        <v>3</v>
+      </c>
+      <c r="X80" s="1">
+        <v>5</v>
       </c>
       <c r="Y80" s="1" t="s">
         <v>100</v>
@@ -17298,6 +17307,7 @@
   </sheetData>
   <autoFilter ref="A1:AJ85" xr:uid="{98088FFF-07F4-4BB5-BAC5-BF377CA38131}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>